<commit_message>
Clean up warnings and extraneous messages
Fix incorrect forumula on some input files.
Add suppressMessages to all "read_" functions.
Use dplyr::all_of for less ambiguous selects
Explicitly set .groups on summarise
Update documentation and set to rebuild docs in RStudio
</commit_message>
<xml_diff>
--- a/inst/extdata/C_Sample_Input_Simple.xlsx
+++ b/inst/extdata/C_Sample_Input_Simple.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="47">
   <si>
     <t xml:space="preserve">Compound</t>
   </si>
@@ -94,24 +94,6 @@
     <t xml:space="preserve">C6H14O12P2</t>
   </si>
   <si>
-    <t xml:space="preserve">C6H14O12P3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C6H14O12P4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C6H14O12P5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C6H14O12P6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C6H14O12P7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C6H14O12P8</t>
-  </si>
-  <si>
     <t xml:space="preserve">C13-label-6</t>
   </si>
   <si>
@@ -163,45 +145,15 @@
     <t xml:space="preserve">C21H29N7O14P2</t>
   </si>
   <si>
-    <t xml:space="preserve">C21H29N7O14P3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C21H29N7O14P4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C21H29N7O14P5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C21H29N7O14P6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C21H29N7O14P7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C21H29N7O14P8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C21H29N7O14P9</t>
-  </si>
-  <si>
     <t xml:space="preserve">C13-label-7</t>
   </si>
   <si>
-    <t xml:space="preserve">C21H29N7O14P10</t>
-  </si>
-  <si>
     <t xml:space="preserve">C13-label-8</t>
   </si>
   <si>
-    <t xml:space="preserve">C21H29N7O14P11</t>
-  </si>
-  <si>
     <t xml:space="preserve">C13-label-9</t>
   </si>
   <si>
-    <t xml:space="preserve">C21H29N7O14P12</t>
-  </si>
-  <si>
     <t xml:space="preserve">C13-label-10</t>
   </si>
   <si>
@@ -209,36 +161,6 @@
   </si>
   <si>
     <t xml:space="preserve">C21H27N7O14P2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C21H27N7O14P3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C21H27N7O14P4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C21H27N7O14P5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C21H27N7O14P6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C21H27N7O14P7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C21H27N7O14P8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C21H27N7O14P9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C21H27N7O14P10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C21H27N7O14P11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C21H27N7O14P12</t>
   </si>
 </sst>
 </file>
@@ -314,9 +236,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -325,12 +251,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -340,60 +266,59 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L1048576"/>
+  <dimension ref="A1:L71"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.85"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -431,7 +356,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -469,7 +394,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -507,7 +432,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
@@ -545,7 +470,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="0" t="s">
@@ -583,7 +508,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="0" t="s">
@@ -621,7 +546,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="0" t="s">
@@ -659,7 +584,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="0" t="s">
@@ -697,7 +622,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="0" t="s">
@@ -735,7 +660,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="0" t="s">
@@ -773,7 +698,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="0" t="s">
@@ -811,7 +736,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="0" t="s">
@@ -849,11 +774,11 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>15</v>
@@ -887,11 +812,11 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>16</v>
@@ -925,11 +850,11 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>17</v>
@@ -963,11 +888,11 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>18</v>
@@ -1001,11 +926,11 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>19</v>
@@ -1039,14 +964,14 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>318.1</v>
@@ -1077,11 +1002,11 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>31</v>
+      <c r="A20" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>14</v>
@@ -1115,11 +1040,11 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>31</v>
+      <c r="A21" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>15</v>
@@ -1153,11 +1078,11 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>31</v>
+      <c r="A22" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>16</v>
@@ -1191,11 +1116,11 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>33</v>
+      <c r="A23" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>14</v>
@@ -1229,11 +1154,11 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>33</v>
+      <c r="A24" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>15</v>
@@ -1267,11 +1192,11 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>33</v>
+      <c r="A25" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>16</v>
@@ -1305,11 +1230,11 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>33</v>
+      <c r="A26" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>17</v>
@@ -1343,11 +1268,11 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>35</v>
+      <c r="A27" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>14</v>
@@ -1381,11 +1306,11 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>35</v>
+      <c r="A28" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>15</v>
@@ -1419,11 +1344,11 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>35</v>
+      <c r="A29" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>16</v>
@@ -1457,11 +1382,11 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>35</v>
+      <c r="A30" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>17</v>
@@ -1495,11 +1420,11 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>37</v>
+      <c r="A31" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>14</v>
@@ -1533,11 +1458,11 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
-        <v>37</v>
+      <c r="A32" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>15</v>
@@ -1571,11 +1496,11 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>37</v>
+      <c r="A33" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>16</v>
@@ -1609,11 +1534,11 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
-        <v>39</v>
+      <c r="A34" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>14</v>
@@ -1647,11 +1572,11 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>39</v>
+      <c r="A35" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>15</v>
@@ -1685,11 +1610,11 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
-        <v>39</v>
+      <c r="A36" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>16</v>
@@ -1723,11 +1648,11 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
-        <v>39</v>
+      <c r="A37" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>17</v>
@@ -1761,11 +1686,11 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>41</v>
+      <c r="A38" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>14</v>
@@ -1799,11 +1724,11 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
-        <v>41</v>
+      <c r="A39" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>15</v>
@@ -1837,11 +1762,11 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>41</v>
+      <c r="A40" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>16</v>
@@ -1875,11 +1800,11 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
-        <v>41</v>
+      <c r="A41" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>17</v>
@@ -1913,11 +1838,11 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
-        <v>41</v>
+      <c r="A42" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>18</v>
@@ -1951,11 +1876,11 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
-        <v>41</v>
+      <c r="A43" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>19</v>
@@ -1989,11 +1914,11 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
-        <v>43</v>
+      <c r="A44" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>14</v>
@@ -2027,11 +1952,11 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
-        <v>43</v>
+      <c r="A45" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>15</v>
@@ -2065,11 +1990,11 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
-        <v>43</v>
+      <c r="A46" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>16</v>
@@ -2103,11 +2028,11 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
-        <v>43</v>
+      <c r="A47" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>17</v>
@@ -2141,11 +2066,11 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
-        <v>43</v>
+      <c r="A48" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>18</v>
@@ -2179,11 +2104,11 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
-        <v>43</v>
+      <c r="A49" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>19</v>
@@ -2217,11 +2142,11 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
-        <v>45</v>
+      <c r="A50" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>14</v>
@@ -2255,11 +2180,11 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
-        <v>45</v>
+      <c r="A51" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>15</v>
@@ -2293,11 +2218,11 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
-        <v>45</v>
+      <c r="A52" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>16</v>
@@ -2331,11 +2256,11 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
-        <v>45</v>
+      <c r="A53" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>17</v>
@@ -2369,11 +2294,11 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="s">
-        <v>45</v>
+      <c r="A54" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>18</v>
@@ -2407,11 +2332,11 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
-        <v>45</v>
+      <c r="A55" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>19</v>
@@ -2445,14 +2370,14 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
-        <v>45</v>
+      <c r="A56" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D56" s="0" t="n">
         <v>82076.09</v>
@@ -2483,14 +2408,14 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="s">
-        <v>45</v>
+      <c r="A57" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>40775.71</v>
@@ -2521,14 +2446,14 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
-        <v>45</v>
+      <c r="A58" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>17112.08</v>
@@ -2559,14 +2484,14 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
-        <v>45</v>
+      <c r="A59" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="D59" s="0" t="n">
         <v>4965.55</v>
@@ -2597,14 +2522,14 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
-        <v>45</v>
+      <c r="A60" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D60" s="0" t="n">
         <v>1370.1</v>
@@ -2635,11 +2560,11 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="s">
-        <v>61</v>
+      <c r="A61" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C61" s="0" t="s">
         <v>14</v>
@@ -2673,11 +2598,11 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="s">
-        <v>61</v>
+      <c r="A62" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C62" s="0" t="s">
         <v>15</v>
@@ -2711,11 +2636,11 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="s">
-        <v>61</v>
+      <c r="A63" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C63" s="0" t="s">
         <v>16</v>
@@ -2749,11 +2674,11 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="s">
-        <v>61</v>
+      <c r="A64" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="C64" s="0" t="s">
         <v>17</v>
@@ -2787,11 +2712,11 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
-        <v>61</v>
+      <c r="A65" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="C65" s="0" t="s">
         <v>18</v>
@@ -2825,11 +2750,11 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
-        <v>61</v>
+      <c r="A66" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="C66" s="0" t="s">
         <v>19</v>
@@ -2863,14 +2788,14 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
-        <v>61</v>
+      <c r="A67" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D67" s="0" t="n">
         <v>56787.7</v>
@@ -2901,14 +2826,14 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
-        <v>61</v>
+      <c r="A68" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D68" s="0" t="n">
         <v>32207.16</v>
@@ -2939,14 +2864,14 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
-        <v>61</v>
+      <c r="A69" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D69" s="0" t="n">
         <v>14669.86</v>
@@ -2977,14 +2902,14 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
-        <v>61</v>
+      <c r="A70" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="D70" s="0" t="n">
         <v>3379.79</v>
@@ -3015,14 +2940,14 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="s">
-        <v>61</v>
+      <c r="A71" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D71" s="0" t="n">
         <v>488.7</v>
@@ -3052,18 +2977,6 @@
         <v>1804.9</v>
       </c>
     </row>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>